<commit_message>
fontosabb kényszerek implementálva, tesztelni kell
</commit_message>
<xml_diff>
--- a/import2.xlsx
+++ b/import2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berta\IdeaProjects\SchoolTimeTableM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5242A3-6AE0-4981-AC03-5C79178BBC21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AE6A71-8CBF-4058-9128-0AC57BDF9699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="110">
   <si>
     <t>Tantárgy</t>
   </si>
@@ -370,6 +370,9 @@
   </si>
   <si>
     <t>Ebédlő1</t>
+  </si>
+  <si>
+    <t>ÚT2</t>
   </si>
 </sst>
 </file>
@@ -586,13 +589,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -1092,15 +1095,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2529DACB-EA8E-4534-BF76-718A4B311EF4}">
-  <dimension ref="A1:R17"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:R17"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -1119,7 +1122,7 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>62</v>
       </c>
@@ -1136,7 +1139,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>63</v>
       </c>
@@ -1144,7 +1147,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>64</v>
       </c>
@@ -1152,7 +1155,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>65</v>
       </c>
@@ -1163,7 +1166,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>66</v>
       </c>
@@ -1171,7 +1174,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>67</v>
       </c>
@@ -1223,8 +1226,11 @@
       <c r="R7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>68</v>
       </c>
@@ -1276,8 +1282,11 @@
       <c r="R8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>69</v>
       </c>
@@ -1329,8 +1338,11 @@
       <c r="R9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>70</v>
       </c>
@@ -1382,8 +1394,11 @@
       <c r="R10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>71</v>
       </c>
@@ -1435,8 +1450,11 @@
       <c r="R11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>72</v>
       </c>
@@ -1488,8 +1506,11 @@
       <c r="R12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>73</v>
       </c>
@@ -1541,8 +1562,11 @@
       <c r="R13" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>74</v>
       </c>
@@ -1594,8 +1618,11 @@
       <c r="R14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>108</v>
       </c>
@@ -1603,15 +1630,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="27" t="s">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" s="25" t="s">
         <v>107</v>
       </c>
       <c r="B16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>106</v>
       </c>
@@ -1663,8 +1690,68 @@
       <c r="R17" t="s">
         <v>36</v>
       </c>
+      <c r="S17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" t="s">
+        <v>38</v>
+      </c>
+      <c r="K18" t="s">
+        <v>39</v>
+      </c>
+      <c r="L18" t="s">
+        <v>44</v>
+      </c>
+      <c r="M18" t="s">
+        <v>45</v>
+      </c>
+      <c r="N18" t="s">
+        <v>40</v>
+      </c>
+      <c r="O18" t="s">
+        <v>49</v>
+      </c>
+      <c r="P18" t="s">
+        <v>27</v>
+      </c>
+      <c r="R18" t="s">
+        <v>36</v>
+      </c>
+      <c r="S18" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1688,67 +1775,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="25" t="s">
+      <c r="A1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25" t="s">
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25" t="s">
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25" t="s">
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
-      <c r="AK1" s="25"/>
-      <c r="AL1" s="25" t="s">
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="AM1" s="25"/>
-      <c r="AN1" s="25"/>
-      <c r="AO1" s="25"/>
-      <c r="AP1" s="25"/>
-      <c r="AQ1" s="25"/>
-      <c r="AR1" s="25"/>
-      <c r="AS1" s="25"/>
-      <c r="AT1" s="25"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
+      <c r="AQ1" s="26"/>
+      <c r="AR1" s="26"/>
+      <c r="AS1" s="26"/>
+      <c r="AT1" s="26"/>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
+      <c r="A2" s="27"/>
       <c r="B2" s="2">
         <v>1</v>
       </c>

</xml_diff>